<commit_message>
Added Task examples and profiles
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-DocumentReference.xlsx
+++ b/docs/StructureDefinition-DocumentReference.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-26T11:48:15+00:00</t>
+    <t>2024-02-28T08:09:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1841,17 +1841,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="49.81640625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="48.453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="48.453125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="180.09375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="180.26953125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1860,29 +1860,29 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="35.59375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="71.41015625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="57.5546875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="43.2890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="35.75" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="70.828125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="57.93359375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="42.265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="26.71875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="50.96484375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="26.69140625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="50.64453125" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="255.0" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="82.05078125" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="157.95703125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="33.05078125" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="81.69140625" customWidth="true" bestFit="true"/>
+    <col min="43" max="43" width="155.44140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>